<commit_message>
- change pin assignment - clean-up GPIOs on exit
</commit_message>
<xml_diff>
--- a/doc/pin_assignment.xlsx
+++ b/doc/pin_assignment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="15300" windowHeight="8736"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="15300" windowHeight="8730"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -195,9 +195,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -235,7 +235,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -305,7 +305,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -481,20 +481,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="7.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="8.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="1.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="2" style="2" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="1.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="7.2" customHeight="1">
+    <row r="2" spans="1:7" ht="7.15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -511,7 +513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="7.2" customHeight="1">
+    <row r="3" spans="1:7" ht="7.15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -528,7 +530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="7.2" customHeight="1">
+    <row r="4" spans="1:7" ht="7.15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -544,8 +546,11 @@
       <c r="F4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="7.2" customHeight="1">
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="7.15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -561,11 +566,11 @@
       <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="7.2" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="7.15" customHeight="1">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -579,9 +584,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="7.2" customHeight="1">
+    <row r="7" spans="1:7" ht="7.15" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>6</v>
@@ -596,7 +601,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="7.2" customHeight="1">
+    <row r="8" spans="1:7" ht="7.15" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
@@ -609,8 +617,14 @@
       <c r="F8" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="7.2" customHeight="1">
+      <c r="G8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="7.15" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
@@ -627,7 +641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="7.2" customHeight="1">
+    <row r="10" spans="1:7" ht="7.15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -643,11 +657,8 @@
       <c r="F10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="7.2" customHeight="1">
+    </row>
+    <row r="11" spans="1:7" ht="7.15" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
@@ -660,11 +671,8 @@
       <c r="F11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="7.2" customHeight="1">
+    </row>
+    <row r="12" spans="1:7" ht="7.15" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
@@ -677,11 +685,8 @@
       <c r="F12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="7.2" customHeight="1">
+    </row>
+    <row r="13" spans="1:7" ht="7.15" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
@@ -695,7 +700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="7.2" customHeight="1">
+    <row r="14" spans="1:7" ht="7.15" customHeight="1">
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -707,9 +712,6 @@
       </c>
       <c r="F14" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +726,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -736,7 +738,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- update pin assignment
</commit_message>
<xml_diff>
--- a/doc/pin_assignment.xlsx
+++ b/doc/pin_assignment.xlsx
@@ -482,7 +482,7 @@
   <dimension ref="A2:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="8.25"/>
@@ -498,7 +498,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="7.15" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="3" spans="1:7" ht="7.15" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="4" spans="1:7" ht="7.15" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>4</v>
@@ -547,12 +547,12 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="7.15" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>5</v>
@@ -567,7 +567,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="7.15" customHeight="1">
@@ -586,7 +586,7 @@
     </row>
     <row r="7" spans="1:7" ht="7.15" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>6</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="8" spans="1:7" ht="7.15" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>7</v>
@@ -618,12 +618,12 @@
         <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="7.15" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>8</v>
@@ -638,12 +638,12 @@
         <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="7.15" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>0</v>

</xml_diff>